<commit_message>
Added analytics demo artifacts
</commit_message>
<xml_diff>
--- a/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
+++ b/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="589">
   <si>
     <t>ID</t>
   </si>
@@ -1789,21 +1789,6 @@
   </si>
   <si>
     <t>Human Trafficking, Involuntary Servitude</t>
-  </si>
-  <si>
-    <t>Animal Cruelty</t>
-  </si>
-  <si>
-    <t>26F</t>
-  </si>
-  <si>
-    <t>Identity Theft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hacking/Computer Invasion </t>
-  </si>
-  <si>
-    <t>26G</t>
   </si>
   <si>
     <t>UCROffenseCodeTypeID</t>
@@ -1900,15 +1885,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -5427,10 +5409,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5443,21 +5425,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="C1" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="D1" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -5466,12 +5448,12 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>25</v>
@@ -5480,12 +5462,12 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>27</v>
@@ -5494,12 +5476,12 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="B5" s="2">
         <v>100</v>
@@ -5508,12 +5490,12 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>39</v>
+        <v>111</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>88</v>
@@ -5522,12 +5504,12 @@
         <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>90</v>
@@ -5536,12 +5518,12 @@
         <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>92</v>
@@ -5550,12 +5532,12 @@
         <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>94</v>
@@ -5564,12 +5546,12 @@
         <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B10" s="2">
         <v>120</v>
@@ -5578,12 +5560,12 @@
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>31</v>
@@ -5592,12 +5574,12 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>7</v>
+        <v>132</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>33</v>
@@ -5606,12 +5588,12 @@
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>8</v>
+        <v>133</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>35</v>
@@ -5620,12 +5602,12 @@
         <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>9</v>
+        <v>200</v>
       </c>
       <c r="B14" s="2">
         <v>200</v>
@@ -5634,12 +5616,12 @@
         <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>10</v>
+        <v>210</v>
       </c>
       <c r="B15" s="2">
         <v>210</v>
@@ -5648,12 +5630,12 @@
         <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>11</v>
+        <v>220</v>
       </c>
       <c r="B16" s="2">
         <v>220</v>
@@ -5662,12 +5644,12 @@
         <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>12</v>
+        <v>231</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>40</v>
@@ -5676,12 +5658,12 @@
         <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>13</v>
+        <v>232</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>42</v>
@@ -5690,12 +5672,12 @@
         <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>14</v>
+        <v>233</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>44</v>
@@ -5704,12 +5686,12 @@
         <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>15</v>
+        <v>234</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>46</v>
@@ -5718,12 +5700,12 @@
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>16</v>
+        <v>235</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>48</v>
@@ -5732,12 +5714,12 @@
         <v>49</v>
       </c>
       <c r="D21" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>17</v>
+        <v>236</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>50</v>
@@ -5746,12 +5728,12 @@
         <v>51</v>
       </c>
       <c r="D22" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>18</v>
+        <v>237</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>52</v>
@@ -5760,12 +5742,12 @@
         <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>19</v>
+        <v>238</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>54</v>
@@ -5774,12 +5756,12 @@
         <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>20</v>
+        <v>240</v>
       </c>
       <c r="B25" s="2">
         <v>240</v>
@@ -5788,12 +5770,12 @@
         <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>21</v>
+        <v>250</v>
       </c>
       <c r="B26" s="2">
         <v>250</v>
@@ -5802,12 +5784,12 @@
         <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>22</v>
+        <v>261</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>58</v>
@@ -5816,12 +5798,12 @@
         <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>23</v>
+        <v>262</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>60</v>
@@ -5830,12 +5812,12 @@
         <v>61</v>
       </c>
       <c r="D28" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>24</v>
+        <v>263</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>62</v>
@@ -5844,12 +5826,12 @@
         <v>63</v>
       </c>
       <c r="D29" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>25</v>
+        <v>264</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>64</v>
@@ -5858,12 +5840,12 @@
         <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>26</v>
+        <v>265</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>66</v>
@@ -5872,468 +5854,426 @@
         <v>67</v>
       </c>
       <c r="D31" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>59</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>582</v>
+        <v>270</v>
+      </c>
+      <c r="B32" s="2">
+        <v>270</v>
       </c>
       <c r="C32" t="s">
-        <v>583</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>63</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>585</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>584</v>
+        <v>280</v>
+      </c>
+      <c r="B33" s="2">
+        <v>280</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>27</v>
+        <v>290</v>
       </c>
       <c r="B34" s="2">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>43</v>
-      </c>
-      <c r="B35" s="2">
-        <v>280</v>
+        <v>351</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="D35" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>28</v>
-      </c>
-      <c r="B36" s="2">
-        <v>290</v>
+        <v>352</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D36" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>29</v>
+        <v>361</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" t="s">
-        <v>593</v>
+        <v>98</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>30</v>
+      <c r="A38" s="1">
+        <v>362</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" t="s">
-        <v>73</v>
+        <v>99</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="D38" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>44</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>97</v>
+        <v>370</v>
+      </c>
+      <c r="B39" s="2">
+        <v>370</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>590</v>
+        <v>74</v>
+      </c>
+      <c r="D39" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>45</v>
+      <c r="A40">
+        <v>391</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>100</v>
+        <v>75</v>
+      </c>
+      <c r="C40" t="s">
+        <v>76</v>
       </c>
       <c r="D40" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>31</v>
-      </c>
-      <c r="B41" s="2">
-        <v>370</v>
+        <v>392</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D41" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>32</v>
+        <v>393</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D42" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>33</v>
+        <v>394</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D43" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>34</v>
+        <v>401</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D44" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>35</v>
+        <v>402</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D45" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>36</v>
+        <v>403</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>83</v>
+        <v>575</v>
       </c>
       <c r="C46" t="s">
-        <v>84</v>
+        <v>576</v>
       </c>
       <c r="D46" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>37</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>85</v>
+        <v>510</v>
+      </c>
+      <c r="B47" s="2">
+        <v>510</v>
       </c>
       <c r="C47" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D47" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>60</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>575</v>
+        <v>520</v>
+      </c>
+      <c r="B48" s="2">
+        <v>520</v>
       </c>
       <c r="C48" t="s">
-        <v>576</v>
+        <v>101</v>
       </c>
       <c r="D48" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>38</v>
-      </c>
-      <c r="B49" s="2">
-        <v>510</v>
+        <v>641</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>577</v>
       </c>
       <c r="C49" t="s">
-        <v>87</v>
+        <v>578</v>
       </c>
       <c r="D49" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>46</v>
-      </c>
-      <c r="B50" s="2">
-        <v>520</v>
+        <v>642</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>579</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
+        <v>580</v>
       </c>
       <c r="D50" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>61</v>
+        <v>901</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>577</v>
+        <v>102</v>
       </c>
       <c r="C51" t="s">
-        <v>578</v>
+        <v>103</v>
       </c>
       <c r="D51" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>62</v>
+        <v>902</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>579</v>
+        <v>104</v>
       </c>
       <c r="C52" t="s">
-        <v>580</v>
+        <v>105</v>
       </c>
       <c r="D52" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>58</v>
-      </c>
-      <c r="B53" s="5">
-        <v>720</v>
+        <v>903</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="C53" t="s">
-        <v>581</v>
+        <v>107</v>
       </c>
       <c r="D53" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>47</v>
+        <v>904</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C54" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D54" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>48</v>
+        <v>905</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C55" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="D55" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>49</v>
+        <v>906</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C56" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D56" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>50</v>
+        <v>907</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C57" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D57" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>51</v>
+        <v>908</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C58" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D58" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>52</v>
+        <v>909</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D59" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>53</v>
+        <v>910</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D60" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>54</v>
+        <v>990</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C61" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D61" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>55</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C62" t="s">
-        <v>119</v>
-      </c>
-      <c r="D62" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>56</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C63" t="s">
-        <v>121</v>
-      </c>
-      <c r="D63" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>57</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C64" t="s">
-        <v>123</v>
-      </c>
-      <c r="D64" t="s">
         <v>252</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Clean up Agency table and add AgencyType
</commit_message>
<xml_diff>
--- a/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
+++ b/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="30525" yWindow="465" windowWidth="24720" windowHeight="14355" tabRatio="705" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="30525" yWindow="465" windowWidth="24720" windowHeight="14355" tabRatio="705" firstSheet="25" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="MultipleArresteeSegmentsIndicat" sheetId="27" r:id="rId27"/>
     <sheet name="ArresteeWasArmedWithType" sheetId="28" r:id="rId28"/>
     <sheet name="DispositionOfArresteeUnder18Typ" sheetId="29" r:id="rId29"/>
+    <sheet name="AgencyType" sheetId="30" r:id="rId30"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="654">
   <si>
     <t>Table</t>
   </si>
@@ -1955,6 +1956,60 @@
   </si>
   <si>
     <t>98</t>
+  </si>
+  <si>
+    <t>Covered by another agency</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>University or college</t>
+  </si>
+  <si>
+    <t>State Police</t>
+  </si>
+  <si>
+    <t>Special Agency</t>
+  </si>
+  <si>
+    <t>Other state agencies</t>
+  </si>
+  <si>
+    <t>Tribal agencies</t>
+  </si>
+  <si>
+    <t>Federal agencies</t>
+  </si>
+  <si>
+    <t>AgencyType</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -2354,10 +2409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2596,6 +2651,14 @@
       </c>
       <c r="B29" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>645</v>
+      </c>
+      <c r="B30" t="s">
+        <v>645</v>
       </c>
     </row>
   </sheetData>
@@ -4187,7 +4250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -6377,6 +6440,146 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9" style="1"/>
+    <col min="3" max="3" width="23.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>646</v>
+      </c>
+      <c r="C2" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>647</v>
+      </c>
+      <c r="C3" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>648</v>
+      </c>
+      <c r="C4" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="C5" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>650</v>
+      </c>
+      <c r="C6" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="C7" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="C8" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="C9" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="C10" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>99</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="C11" t="s">
+        <v>277</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G64"/>

</xml_diff>

<commit_message>
Fix code table value length issues
</commit_message>
<xml_diff>
--- a/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
+++ b/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="30525" yWindow="465" windowWidth="24720" windowHeight="14355" tabRatio="705" firstSheet="25" activeTab="29"/>
+    <workbookView xWindow="30525" yWindow="465" windowWidth="24720" windowHeight="14355" tabRatio="705" firstSheet="13" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -1496,9 +1496,6 @@
     <t>Firearm (type not stated)</t>
   </si>
   <si>
-    <t>Lethal Cutting Instrument (e.g., switchblade knife or martial arts stars)</t>
-  </si>
-  <si>
     <t>Club/Blackjack/Brass Knuckles</t>
   </si>
   <si>
@@ -2010,6 +2007,9 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>Lethal Cutting Instrument</t>
   </si>
 </sst>
 </file>
@@ -2551,7 +2551,7 @@
     </row>
     <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B17" t="s">
         <v>27</v>
@@ -2655,10 +2655,10 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B30" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -2695,7 +2695,7 @@
         <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2709,7 +2709,7 @@
         <v>279</v>
       </c>
       <c r="D2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2723,7 +2723,7 @@
         <v>280</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2737,7 +2737,7 @@
         <v>281</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2751,7 +2751,7 @@
         <v>282</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2765,7 +2765,7 @@
         <v>283</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2779,7 +2779,7 @@
         <v>284</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2793,7 +2793,7 @@
         <v>285</v>
       </c>
       <c r="D8" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2807,7 +2807,7 @@
         <v>286</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2821,7 +2821,7 @@
         <v>287</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2835,7 +2835,7 @@
         <v>288</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2849,7 +2849,7 @@
         <v>289</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2863,7 +2863,7 @@
         <v>290</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2877,7 +2877,7 @@
         <v>291</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2891,7 +2891,7 @@
         <v>292</v>
       </c>
       <c r="D15" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2905,7 +2905,7 @@
         <v>293</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2919,7 +2919,7 @@
         <v>294</v>
       </c>
       <c r="D17" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2933,7 +2933,7 @@
         <v>295</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2947,7 +2947,7 @@
         <v>296</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2961,7 +2961,7 @@
         <v>297</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2975,7 +2975,7 @@
         <v>298</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2989,7 +2989,7 @@
         <v>299</v>
       </c>
       <c r="D22" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3003,7 +3003,7 @@
         <v>300</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3017,7 +3017,7 @@
         <v>301</v>
       </c>
       <c r="D24" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3031,7 +3031,7 @@
         <v>302</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3045,7 +3045,7 @@
         <v>303</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3059,7 +3059,7 @@
         <v>304</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3140,7 +3140,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3173,7 +3173,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3184,7 +3184,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3195,7 +3195,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3203,7 +3203,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C9" t="s">
         <v>277</v>
@@ -3293,7 +3293,7 @@
         <v>165</v>
       </c>
       <c r="C6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3304,7 +3304,7 @@
         <v>167</v>
       </c>
       <c r="C7" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3315,7 +3315,7 @@
         <v>169</v>
       </c>
       <c r="C8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3326,7 +3326,7 @@
         <v>171</v>
       </c>
       <c r="C9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3337,7 +3337,7 @@
         <v>173</v>
       </c>
       <c r="C10" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3359,7 +3359,7 @@
         <v>177</v>
       </c>
       <c r="C12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3370,7 +3370,7 @@
         <v>179</v>
       </c>
       <c r="C13" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3381,7 +3381,7 @@
         <v>181</v>
       </c>
       <c r="C14" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3392,7 +3392,7 @@
         <v>183</v>
       </c>
       <c r="C15" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3403,7 +3403,7 @@
         <v>185</v>
       </c>
       <c r="C16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3414,7 +3414,7 @@
         <v>187</v>
       </c>
       <c r="C17" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3425,7 +3425,7 @@
         <v>189</v>
       </c>
       <c r="C18" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3436,7 +3436,7 @@
         <v>191</v>
       </c>
       <c r="C19" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3447,7 +3447,7 @@
         <v>192</v>
       </c>
       <c r="C20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3458,7 +3458,7 @@
         <v>194</v>
       </c>
       <c r="C21" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3469,7 +3469,7 @@
         <v>196</v>
       </c>
       <c r="C22" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3480,7 +3480,7 @@
         <v>198</v>
       </c>
       <c r="C23" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3491,7 +3491,7 @@
         <v>200</v>
       </c>
       <c r="C24" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3502,7 +3502,7 @@
         <v>202</v>
       </c>
       <c r="C25" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3513,7 +3513,7 @@
         <v>204</v>
       </c>
       <c r="C26" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3524,7 +3524,7 @@
         <v>312</v>
       </c>
       <c r="C27" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3535,7 +3535,7 @@
         <v>313</v>
       </c>
       <c r="C28" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3546,7 +3546,7 @@
         <v>314</v>
       </c>
       <c r="C29" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3557,7 +3557,7 @@
         <v>315</v>
       </c>
       <c r="C30" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3568,7 +3568,7 @@
         <v>316</v>
       </c>
       <c r="C31" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3579,7 +3579,7 @@
         <v>317</v>
       </c>
       <c r="C32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3590,7 +3590,7 @@
         <v>318</v>
       </c>
       <c r="C33" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3601,7 +3601,7 @@
         <v>319</v>
       </c>
       <c r="C34" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3612,7 +3612,7 @@
         <v>320</v>
       </c>
       <c r="C35" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3623,7 +3623,7 @@
         <v>321</v>
       </c>
       <c r="C36" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3634,7 +3634,7 @@
         <v>322</v>
       </c>
       <c r="C37" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3645,7 +3645,7 @@
         <v>206</v>
       </c>
       <c r="C38" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3656,7 +3656,7 @@
         <v>208</v>
       </c>
       <c r="C39" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3667,7 +3667,7 @@
         <v>210</v>
       </c>
       <c r="C40" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3678,7 +3678,7 @@
         <v>214</v>
       </c>
       <c r="C41" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3689,7 +3689,7 @@
         <v>216</v>
       </c>
       <c r="C42" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3700,7 +3700,7 @@
         <v>323</v>
       </c>
       <c r="C43" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3711,7 +3711,7 @@
         <v>218</v>
       </c>
       <c r="C44" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3733,7 +3733,7 @@
         <v>222</v>
       </c>
       <c r="C46" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3755,7 +3755,7 @@
         <v>226</v>
       </c>
       <c r="C48" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3777,7 +3777,7 @@
         <v>326</v>
       </c>
       <c r="C50" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3799,7 +3799,7 @@
         <v>329</v>
       </c>
       <c r="C52" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3810,7 +3810,7 @@
         <v>330</v>
       </c>
       <c r="C53" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3821,7 +3821,7 @@
         <v>331</v>
       </c>
       <c r="C54" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3832,7 +3832,7 @@
         <v>332</v>
       </c>
       <c r="C55" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3843,7 +3843,7 @@
         <v>333</v>
       </c>
       <c r="C56" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3854,7 +3854,7 @@
         <v>334</v>
       </c>
       <c r="C57" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3865,7 +3865,7 @@
         <v>335</v>
       </c>
       <c r="C58" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3876,7 +3876,7 @@
         <v>336</v>
       </c>
       <c r="C59" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3898,7 +3898,7 @@
         <v>339</v>
       </c>
       <c r="C61" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3909,7 +3909,7 @@
         <v>340</v>
       </c>
       <c r="C62" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3920,7 +3920,7 @@
         <v>341</v>
       </c>
       <c r="C63" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3953,7 +3953,7 @@
         <v>345</v>
       </c>
       <c r="C66" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3964,7 +3964,7 @@
         <v>346</v>
       </c>
       <c r="C67" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3975,7 +3975,7 @@
         <v>347</v>
       </c>
       <c r="C68" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3994,7 +3994,7 @@
         <v>98</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C70" t="s">
         <v>278</v>
@@ -4039,7 +4039,7 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4050,7 +4050,7 @@
         <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4061,7 +4061,7 @@
         <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4072,7 +4072,7 @@
         <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4083,7 +4083,7 @@
         <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4094,7 +4094,7 @@
         <v>246</v>
       </c>
       <c r="C7" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4105,7 +4105,7 @@
         <v>261</v>
       </c>
       <c r="C8" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4116,7 +4116,7 @@
         <v>349</v>
       </c>
       <c r="C9" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4149,7 +4149,7 @@
         <v>352</v>
       </c>
       <c r="C12" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4160,7 +4160,7 @@
         <v>353</v>
       </c>
       <c r="C13" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4171,7 +4171,7 @@
         <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4182,7 +4182,7 @@
         <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4193,7 +4193,7 @@
         <v>252</v>
       </c>
       <c r="C16" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4204,7 +4204,7 @@
         <v>254</v>
       </c>
       <c r="C17" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4226,7 +4226,7 @@
         <v>355</v>
       </c>
       <c r="C19" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -4234,7 +4234,7 @@
         <v>98</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C20" t="s">
         <v>278</v>
@@ -4407,7 +4407,7 @@
         <v>98</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C14" t="s">
         <v>278</v>
@@ -4492,7 +4492,7 @@
         <v>353</v>
       </c>
       <c r="C6" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4577,7 +4577,7 @@
         <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4810,7 +4810,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C9" t="s">
         <v>277</v>
@@ -4851,7 +4851,7 @@
         <v>246</v>
       </c>
       <c r="C2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4862,7 +4862,7 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4886,11 +4886,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="35.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -4911,7 +4914,7 @@
         <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4922,7 +4925,7 @@
         <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4933,7 +4936,7 @@
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4944,7 +4947,7 @@
         <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4955,7 +4958,7 @@
         <v>254</v>
       </c>
       <c r="C6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5062,7 +5065,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C7" t="s">
         <v>277</v>
@@ -5114,7 +5117,7 @@
         <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5292,7 +5295,7 @@
         <v>169</v>
       </c>
       <c r="C8" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5421,7 +5424,7 @@
         <v>98</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C20" t="s">
         <v>278</v>
@@ -5539,7 +5542,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C9" t="s">
         <v>277</v>
@@ -5583,7 +5586,7 @@
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5594,7 +5597,7 @@
         <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5605,7 +5608,7 @@
         <v>353</v>
       </c>
       <c r="C4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5616,7 +5619,7 @@
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5638,7 +5641,7 @@
         <v>252</v>
       </c>
       <c r="C7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5649,7 +5652,7 @@
         <v>256</v>
       </c>
       <c r="C8" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5660,7 +5663,7 @@
         <v>258</v>
       </c>
       <c r="C9" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5668,7 +5671,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C10" t="s">
         <v>277</v>
@@ -5745,7 +5748,7 @@
         <v>464</v>
       </c>
       <c r="C5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5822,7 +5825,7 @@
         <v>471</v>
       </c>
       <c r="C12" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5995,7 +5998,7 @@
         <v>98</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C28" t="s">
         <v>278</v>
@@ -6042,7 +6045,7 @@
         <v>252</v>
       </c>
       <c r="C2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6053,7 +6056,7 @@
         <v>383</v>
       </c>
       <c r="C3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6064,7 +6067,7 @@
         <v>256</v>
       </c>
       <c r="C4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -6072,7 +6075,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C5" t="s">
         <v>277</v>
@@ -6149,7 +6152,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6242,7 +6245,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>482</v>
+        <v>653</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6253,7 +6256,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6261,7 +6264,7 @@
         <v>999</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>524</v>
+        <v>348</v>
       </c>
       <c r="C10" t="s">
         <v>277</v>
@@ -6305,7 +6308,7 @@
         <v>349</v>
       </c>
       <c r="C2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6316,7 +6319,7 @@
         <v>354</v>
       </c>
       <c r="C3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -6324,7 +6327,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C4" t="s">
         <v>277</v>
@@ -6376,7 +6379,7 @@
         <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6387,7 +6390,7 @@
         <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6398,7 +6401,7 @@
         <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6409,7 +6412,7 @@
         <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6428,7 +6431,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C8" t="s">
         <v>277</v>
@@ -6444,7 +6447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -6470,10 +6473,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -6481,10 +6484,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -6492,10 +6495,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C4" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -6503,10 +6506,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6514,10 +6517,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6525,10 +6528,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6536,10 +6539,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C8" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6547,10 +6550,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C9" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6558,10 +6561,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C10" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6569,7 +6572,7 @@
         <v>99</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C11" t="s">
         <v>277</v>
@@ -6609,16 +6612,16 @@
         <v>36</v>
       </c>
       <c r="D1" t="s">
+        <v>495</v>
+      </c>
+      <c r="E1" t="s">
         <v>496</v>
       </c>
-      <c r="E1" t="s">
-        <v>497</v>
-      </c>
       <c r="F1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6632,16 +6635,16 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6655,16 +6658,16 @@
         <v>55</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E3" t="s">
         <v>276</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6678,16 +6681,16 @@
         <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6701,7 +6704,7 @@
         <v>58</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>276</v>
@@ -6710,7 +6713,7 @@
         <v>58</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6724,16 +6727,16 @@
         <v>59</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6747,16 +6750,16 @@
         <v>61</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6770,16 +6773,16 @@
         <v>63</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6793,16 +6796,16 @@
         <v>65</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6816,16 +6819,16 @@
         <v>66</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F10" t="s">
         <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6839,7 +6842,7 @@
         <v>67</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>276</v>
@@ -6848,7 +6851,7 @@
         <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6862,16 +6865,16 @@
         <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>68</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6885,16 +6888,16 @@
         <v>70</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6908,16 +6911,16 @@
         <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6931,16 +6934,16 @@
         <v>74</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6954,16 +6957,16 @@
         <v>76</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6977,16 +6980,16 @@
         <v>78</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7000,16 +7003,16 @@
         <v>80</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7023,16 +7026,16 @@
         <v>82</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7046,16 +7049,16 @@
         <v>84</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7069,16 +7072,16 @@
         <v>85</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7092,7 +7095,7 @@
         <v>86</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>276</v>
@@ -7101,7 +7104,7 @@
         <v>86</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7115,16 +7118,16 @@
         <v>88</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F23" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7138,16 +7141,16 @@
         <v>90</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7161,16 +7164,16 @@
         <v>92</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7184,16 +7187,16 @@
         <v>94</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7207,16 +7210,16 @@
         <v>96</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7230,7 +7233,7 @@
         <v>97</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>276</v>
@@ -7239,7 +7242,7 @@
         <v>97</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7253,7 +7256,7 @@
         <v>98</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>276</v>
@@ -7262,7 +7265,7 @@
         <v>98</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7276,16 +7279,16 @@
         <v>100</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F30" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G30" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7299,16 +7302,16 @@
         <v>102</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7322,7 +7325,7 @@
         <v>103</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>276</v>
@@ -7331,7 +7334,7 @@
         <v>103</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7345,16 +7348,16 @@
         <v>105</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F33" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7368,16 +7371,16 @@
         <v>107</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7391,16 +7394,16 @@
         <v>109</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7414,16 +7417,16 @@
         <v>111</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7437,16 +7440,16 @@
         <v>113</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F37" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7460,16 +7463,16 @@
         <v>115</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7483,7 +7486,7 @@
         <v>116</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>276</v>
@@ -7492,7 +7495,7 @@
         <v>116</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7506,16 +7509,16 @@
         <v>118</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F40" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G40" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7529,16 +7532,16 @@
         <v>120</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7552,16 +7555,16 @@
         <v>122</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7575,16 +7578,16 @@
         <v>124</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7598,7 +7601,7 @@
         <v>125</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>276</v>
@@ -7607,7 +7610,7 @@
         <v>125</v>
       </c>
       <c r="G44" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7621,16 +7624,16 @@
         <v>127</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F45" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G45" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7644,16 +7647,16 @@
         <v>129</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G46" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7667,7 +7670,7 @@
         <v>130</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>276</v>
@@ -7676,7 +7679,7 @@
         <v>130</v>
       </c>
       <c r="G47" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7690,16 +7693,16 @@
         <v>132</v>
       </c>
       <c r="D48" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F48" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G48" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7713,16 +7716,16 @@
         <v>134</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G49" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7736,16 +7739,16 @@
         <v>136</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7759,16 +7762,16 @@
         <v>138</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7782,16 +7785,16 @@
         <v>140</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7805,16 +7808,16 @@
         <v>142</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7828,16 +7831,16 @@
         <v>144</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7851,16 +7854,16 @@
         <v>146</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7874,16 +7877,16 @@
         <v>148</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G56" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7897,16 +7900,16 @@
         <v>150</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G57" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7920,13 +7923,13 @@
         <v>152</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G58" t="s">
         <v>152</v>
@@ -7940,19 +7943,19 @@
         <v>720</v>
       </c>
       <c r="C59" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G59" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -7960,22 +7963,22 @@
         <v>702</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C60" t="s">
         <v>493</v>
       </c>
-      <c r="C60" t="s">
-        <v>494</v>
-      </c>
       <c r="D60" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G60" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -7983,22 +7986,22 @@
         <v>403</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C61" t="s">
         <v>486</v>
       </c>
-      <c r="C61" t="s">
-        <v>487</v>
-      </c>
       <c r="D61" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G61" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -8006,22 +8009,22 @@
         <v>641</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C62" t="s">
         <v>488</v>
       </c>
-      <c r="C62" t="s">
-        <v>489</v>
-      </c>
       <c r="D62" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F62" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G62" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -8029,22 +8032,22 @@
         <v>642</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C63" t="s">
         <v>490</v>
       </c>
-      <c r="C63" t="s">
-        <v>491</v>
-      </c>
       <c r="D63" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>276</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G63" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -8052,7 +8055,7 @@
         <v>999</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C64" t="s">
         <v>277</v>
@@ -8149,7 +8152,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C6" t="s">
         <v>278</v>
@@ -8381,7 +8384,7 @@
         <v>191</v>
       </c>
       <c r="C19" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8749,7 +8752,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C4" t="s">
         <v>277</v>
@@ -8804,7 +8807,7 @@
         <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8892,7 +8895,7 @@
         <v>261</v>
       </c>
       <c r="C11" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8903,7 +8906,7 @@
         <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -8911,7 +8914,7 @@
         <v>99</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C13" t="s">
         <v>277</v>

</xml_diff>

<commit_message>
Make all the Unknown entries' pkId to be 99999 and Blank entries' to be 99998.
</commit_message>
<xml_diff>
--- a/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
+++ b/tools/r-packages/nibrs/inst/raw/NIBRSCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22100" yWindow="1380" windowWidth="20480" windowHeight="12400" tabRatio="705" firstSheet="27" activeTab="29"/>
+    <workbookView xWindow="1620" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="705" firstSheet="25" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="655">
   <si>
     <t>Table</t>
   </si>
@@ -1940,9 +1940,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>98</t>
-  </si>
-  <si>
     <t>Covered by another agency</t>
   </si>
   <si>
@@ -2013,6 +2010,9 @@
   </si>
   <si>
     <t>Blank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -2067,9 +2067,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2097,7 +2109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="28">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2105,6 +2117,12 @@
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2112,6 +2130,12 @@
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
@@ -2658,10 +2682,10 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B30" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
   </sheetData>
@@ -2683,7 +2707,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3086,7 +3110,7 @@
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1">
       <c r="A29" s="1">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B29">
         <v>99</v>
@@ -3100,16 +3124,16 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B30" t="s">
+        <v>652</v>
+      </c>
+      <c r="C30" t="s">
         <v>653</v>
       </c>
-      <c r="C30" t="s">
-        <v>654</v>
-      </c>
       <c r="D30" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -3128,7 +3152,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3227,10 +3251,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1">
       <c r="A9">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>525</v>
+        <v>629</v>
       </c>
       <c r="C9" t="s">
         <v>274</v>
@@ -3238,13 +3262,13 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C10" t="s">
         <v>653</v>
-      </c>
-      <c r="C10" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -3263,7 +3287,7 @@
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4023,7 +4047,7 @@
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1">
       <c r="A69">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>345</v>
@@ -4034,13 +4058,13 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>98</v>
+        <v>99998</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>630</v>
+        <v>652</v>
       </c>
       <c r="C70" t="s">
-        <v>275</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -4059,7 +4083,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4257,7 +4281,7 @@
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B18" t="s">
         <v>255</v>
@@ -4279,13 +4303,13 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>98</v>
+        <v>99998</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>629</v>
+        <v>652</v>
       </c>
       <c r="C20" t="s">
-        <v>275</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -4301,10 +4325,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4446,7 +4470,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>345</v>
@@ -4457,24 +4481,13 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>98</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>630</v>
+        <v>99998</v>
+      </c>
+      <c r="B14" t="s">
+        <v>652</v>
       </c>
       <c r="C14" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>99999</v>
-      </c>
-      <c r="B15" t="s">
         <v>653</v>
-      </c>
-      <c r="C15" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -4493,7 +4506,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4602,7 +4615,7 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1">
       <c r="A10">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B10" t="s">
         <v>255</v>
@@ -4613,13 +4626,13 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B11" t="s">
+        <v>652</v>
+      </c>
+      <c r="C11" t="s">
         <v>653</v>
-      </c>
-      <c r="C11" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -4638,7 +4651,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4780,7 +4793,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>345</v>
@@ -4791,13 +4804,13 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B14" t="s">
+        <v>652</v>
+      </c>
+      <c r="C14" t="s">
         <v>653</v>
-      </c>
-      <c r="C14" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -4816,7 +4829,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4914,7 +4927,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>525</v>
@@ -4925,13 +4938,13 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B10" t="s">
+        <v>652</v>
+      </c>
+      <c r="C10" t="s">
         <v>653</v>
-      </c>
-      <c r="C10" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -4950,7 +4963,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4990,7 +5003,7 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1">
       <c r="A4">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B4" t="s">
         <v>255</v>
@@ -5001,13 +5014,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B5" t="s">
+        <v>652</v>
+      </c>
+      <c r="C5" t="s">
         <v>653</v>
-      </c>
-      <c r="C5" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5026,7 +5039,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5102,7 +5115,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1">
       <c r="A7">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B7" t="s">
         <v>255</v>
@@ -5113,13 +5126,13 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B8" t="s">
+        <v>652</v>
+      </c>
+      <c r="C8" t="s">
         <v>653</v>
-      </c>
-      <c r="C8" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5141,7 +5154,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5217,7 +5230,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>525</v>
@@ -5228,13 +5241,13 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B8" t="s">
+        <v>652</v>
+      </c>
+      <c r="C8" t="s">
         <v>653</v>
-      </c>
-      <c r="C8" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5253,7 +5266,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5293,7 +5306,7 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1">
       <c r="A4">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B4" t="s">
         <v>255</v>
@@ -5304,13 +5317,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B5" t="s">
+        <v>652</v>
+      </c>
+      <c r="C5" t="s">
         <v>653</v>
-      </c>
-      <c r="C5" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5329,7 +5342,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5369,7 +5382,7 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1">
       <c r="A4">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B4" t="s">
         <v>255</v>
@@ -5380,13 +5393,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B5" t="s">
+        <v>652</v>
+      </c>
+      <c r="C5" t="s">
         <v>653</v>
-      </c>
-      <c r="C5" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5402,10 +5415,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5613,7 +5626,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>345</v>
@@ -5624,24 +5637,13 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>98</v>
+        <v>99998</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>630</v>
+        <v>652</v>
       </c>
       <c r="C20" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>99999</v>
-      </c>
-      <c r="B21" t="s">
         <v>653</v>
-      </c>
-      <c r="C21" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5660,7 +5662,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5758,29 +5760,29 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>525</v>
+        <v>99998</v>
+      </c>
+      <c r="B9" t="s">
+        <v>652</v>
       </c>
       <c r="C9" t="s">
-        <v>274</v>
+        <v>653</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
         <v>99999</v>
       </c>
-      <c r="B10" t="s">
-        <v>653</v>
+      <c r="B10" s="6" t="s">
+        <v>525</v>
       </c>
       <c r="C10" t="s">
-        <v>654</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5794,7 +5796,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5903,29 +5905,29 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>525</v>
+        <v>99998</v>
+      </c>
+      <c r="B10" t="s">
+        <v>652</v>
       </c>
       <c r="C10" t="s">
-        <v>274</v>
+        <v>653</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
         <v>99999</v>
       </c>
-      <c r="B11" t="s">
-        <v>653</v>
+      <c r="B11" s="6" t="s">
+        <v>525</v>
       </c>
       <c r="C11" t="s">
-        <v>654</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5936,10 +5938,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6235,7 +6237,7 @@
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1">
       <c r="A27">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B27" t="s">
         <v>459</v>
@@ -6246,24 +6248,13 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>98</v>
+        <v>99998</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>630</v>
+        <v>654</v>
       </c>
       <c r="C28" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29">
-        <v>99999</v>
-      </c>
-      <c r="B29" t="s">
         <v>653</v>
-      </c>
-      <c r="C29" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -6284,8 +6275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6337,31 +6328,31 @@
         <v>501</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>525</v>
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="1">
+        <v>99998</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>652</v>
       </c>
       <c r="C5" t="s">
-        <v>274</v>
+        <v>653</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
         <v>99999</v>
       </c>
-      <c r="B6" t="s">
-        <v>653</v>
+      <c r="B6" s="6" t="s">
+        <v>525</v>
       </c>
       <c r="C6" t="s">
-        <v>654</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6375,7 +6366,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6429,13 +6420,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B5" t="s">
+        <v>652</v>
+      </c>
+      <c r="C5" t="s">
         <v>653</v>
-      </c>
-      <c r="C5" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -6454,7 +6445,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6547,7 +6538,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1">
@@ -6563,29 +6554,29 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>999</v>
+        <v>99998</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>345</v>
+        <v>652</v>
       </c>
       <c r="C10" t="s">
-        <v>274</v>
+        <v>653</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
         <v>99999</v>
       </c>
-      <c r="B11" t="s">
-        <v>653</v>
+      <c r="B11" s="6" t="s">
+        <v>345</v>
       </c>
       <c r="C11" t="s">
-        <v>654</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6599,7 +6590,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6642,29 +6633,29 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>9</v>
+        <v>99998</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>525</v>
+        <v>652</v>
       </c>
       <c r="C4" t="s">
-        <v>274</v>
+        <v>653</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
         <v>99999</v>
       </c>
-      <c r="B5" t="s">
-        <v>653</v>
+      <c r="B5" s="3">
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>654</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6678,7 +6669,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6765,7 +6756,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>525</v>
@@ -6776,13 +6767,13 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B9" t="s">
+        <v>652</v>
+      </c>
+      <c r="C9" t="s">
         <v>653</v>
-      </c>
-      <c r="C9" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -6798,10 +6789,10 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6826,10 +6817,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -6837,10 +6828,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -6848,10 +6839,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -6859,10 +6850,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C5" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -6870,10 +6861,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -6881,10 +6872,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -6892,10 +6883,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C8" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -6903,10 +6894,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C9" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -6917,17 +6908,28 @@
         <v>629</v>
       </c>
       <c r="C10" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>99</v>
+        <v>638</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="1" customFormat="1">
+      <c r="A11" s="1">
+        <v>99998</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>99999</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>274</v>
       </c>
     </row>
@@ -6946,7 +6948,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6990,7 +6992,7 @@
         <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D2" t="s">
         <v>494</v>
@@ -6999,7 +7001,7 @@
         <v>496</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G2" t="s">
         <v>521</v>
@@ -7013,7 +7015,7 @@
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>494</v>
@@ -7022,7 +7024,7 @@
         <v>273</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>521</v>
@@ -7036,7 +7038,7 @@
         <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>494</v>
@@ -7045,7 +7047,7 @@
         <v>273</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>522</v>
@@ -8410,7 +8412,7 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64">
-        <v>999</v>
+        <v>99999</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>519</v>
@@ -8433,25 +8435,25 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C65" t="s">
         <v>653</v>
       </c>
-      <c r="C65" t="s">
-        <v>654</v>
-      </c>
       <c r="D65" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E65" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F65" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G65" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -8470,10 +8472,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8538,13 +8540,24 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>525</v>
       </c>
       <c r="C6" t="s">
-        <v>275</v>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>99998</v>
+      </c>
+      <c r="B7" t="s">
+        <v>652</v>
+      </c>
+      <c r="C7" t="s">
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -8562,8 +8575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView topLeftCell="C30" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9080,7 +9093,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>345</v>
@@ -9091,13 +9104,13 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C48" t="s">
         <v>653</v>
-      </c>
-      <c r="C48" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -9116,7 +9129,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9159,7 +9172,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>9</v>
+        <v>99999</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>525</v>
@@ -9170,13 +9183,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B5" t="s">
+        <v>652</v>
+      </c>
+      <c r="C5" t="s">
         <v>653</v>
-      </c>
-      <c r="C5" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -9195,7 +9208,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9337,7 +9350,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>99</v>
+        <v>99999</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>525</v>
@@ -9348,13 +9361,13 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>99999</v>
+        <v>99998</v>
       </c>
       <c r="B14" t="s">
+        <v>652</v>
+      </c>
+      <c r="C14" t="s">
         <v>653</v>
-      </c>
-      <c r="C14" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -9373,7 +9386,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9559,7 +9572,7 @@
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17">
-        <v>999</v>
+        <v>99999</v>
       </c>
       <c r="B17" s="2">
         <v>95</v>
@@ -9570,13 +9583,13 @@
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18">
-        <v>990</v>
-      </c>
-      <c r="B18" s="2">
-        <v>99</v>
+        <v>99998</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>652</v>
       </c>
       <c r="C18" t="s">
-        <v>275</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>